<commit_message>
Updated QA tests in Prelab file; updated Lab2 report
</commit_message>
<xml_diff>
--- a/lab2/Prelab/Lab2QAtests.xlsx
+++ b/lab2/Prelab/Lab2QAtests.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pierce\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pierce\MPLABXProjects\ECE372\Team\lab2\Prelab\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -254,7 +254,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -262,39 +262,62 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -580,26 +603,27 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B16" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B21" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4:C15"/>
+      <selection pane="bottomRight" sqref="A1:I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.85546875" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
-    <col min="3" max="4" width="19.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" customWidth="1"/>
     <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" customWidth="1"/>
-    <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1"/>
@@ -624,468 +648,469 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="9" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="2" t="s">
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="9" t="s">
         <v>5</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="2" t="s">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="9" t="s">
         <v>32</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="2" t="s">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="1"/>
+      <c r="I6" s="9"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="2" t="s">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="1"/>
+      <c r="I7" s="9"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="2" t="s">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="1"/>
+      <c r="I8" s="9"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="2" t="s">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="1"/>
+      <c r="I9" s="9"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="2" t="s">
+      <c r="A10" s="4"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="I10" s="1"/>
+      <c r="I10" s="9"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="2" t="s">
+      <c r="A11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="I11" s="1"/>
+      <c r="I11" s="9"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="2" t="s">
+      <c r="A12" s="4"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="I12" s="1"/>
+      <c r="I12" s="9"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="2" t="s">
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H13" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="I13" s="1"/>
+      <c r="I13" s="9"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="2" t="s">
+      <c r="A14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H14" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="I14" s="1"/>
+      <c r="I14" s="9"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="1" t="s">
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H15" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I15" s="1"/>
+      <c r="I15" s="9"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1" t="s">
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9" t="s">
         <v>36</v>
       </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
     <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="8" t="s">
+      <c r="A17" s="4"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F17" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1" t="s">
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9" t="s">
         <v>37</v>
       </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
     <row r="18" spans="1:11" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="8" t="s">
+      <c r="A18" s="4"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1" t="s">
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9" t="s">
         <v>38</v>
       </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="1" t="s">
+      <c r="A19" s="4"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
     <row r="20" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
     </row>
     <row r="21" spans="1:11" ht="120" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="C21" s="14"/>
+      <c r="D21" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
     </row>
     <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
     </row>
     <row r="23" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
     </row>
     <row r="24" spans="1:11" ht="105" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>